<commit_message>
update report excel and report pdf
</commit_message>
<xml_diff>
--- a/reports/excel/test-tables.xlsx
+++ b/reports/excel/test-tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richy/www/github/data-keeper/reports/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90695C6-B841-9847-AE8A-80B9BDAE962B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B4139B-B649-2C4B-993B-244C8AEF0C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,16 +48,16 @@
     <t>Age</t>
   </si>
   <si>
-    <t>${table:csv.name}</t>
+    <t>{{item.name}}</t>
   </si>
   <si>
-    <t>${table:csv.age}</t>
+    <t>{{item.age}}</t>
   </si>
   <si>
-    <t>Images</t>
+    <t>{% img item.imageurl %}{% endfor %}</t>
   </si>
   <si>
-    <t>${table:csv.imageurl:image}</t>
+    <t>Images {% for item in csv %}</t>
   </si>
 </sst>
 </file>
@@ -167,6 +167,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>571500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1828800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>2000250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1" descr="xml.jpg">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8563FA52-779B-8D4E-BC16-9CEEF538318E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3987800" y="977900"/>
+          <a:ext cx="1333500" cy="1428750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -512,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="211" customHeight="1" x14ac:dyDescent="0.2">
@@ -523,10 +572,11 @@
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>